<commit_message>
Correct formula for 2019 f1040 Line 14
</commit_message>
<xml_diff>
--- a/Federal/f1040-2019.xlsx
+++ b/Federal/f1040-2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
   <si>
     <t xml:space="preserve">2019 Form 1040</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t xml:space="preserve">Taxable income. Subtract line 11a from line 8b. If zero or less, enter -0-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">Page 2</t>
@@ -287,6 +284,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -308,12 +306,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -433,12 +433,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -466,6 +466,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,7 +486,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -506,7 +510,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,11 +605,11 @@
   </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="59.65"/>
@@ -657,11 +661,11 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
@@ -685,11 +689,11 @@
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
@@ -713,11 +717,11 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
@@ -741,11 +745,11 @@
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
@@ -769,11 +773,11 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
@@ -783,11 +787,11 @@
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
@@ -797,11 +801,11 @@
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="2" t="s">
         <v>23</v>
       </c>
@@ -811,11 +815,11 @@
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="2" t="s">
         <v>25</v>
       </c>
@@ -828,11 +832,11 @@
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="2" t="s">
         <v>27</v>
       </c>
@@ -842,11 +846,11 @@
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
@@ -870,37 +874,37 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -914,14 +918,14 @@
       <c r="F22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="2" t="s">
         <v>38</v>
       </c>
@@ -931,14 +935,14 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="2" t="s">
         <v>40</v>
       </c>
@@ -947,56 +951,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="16"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
       <c r="E28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>49</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="6"/>
@@ -1004,225 +1003,225 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F30" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="16" t="n">
-        <f aca="false">MIN(F28-F30,0)</f>
+        <v>51</v>
+      </c>
+      <c r="F31" s="17" t="n">
+        <f aca="false">MAX(F28-F30,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
       <c r="E32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F32" s="16"/>
+        <v>53</v>
+      </c>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
       <c r="E33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="16" t="n">
+        <v>55</v>
+      </c>
+      <c r="F33" s="17" t="n">
         <f aca="false">F31+F32</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
       <c r="E34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="16"/>
+        <v>57</v>
+      </c>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B35" s="8" t="s">
-        <v>61</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="16"/>
+        <v>59</v>
+      </c>
+      <c r="D35" s="17"/>
       <c r="E35" s="6"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="D36" s="17"/>
       <c r="E36" s="6"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>65</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="D37" s="17"/>
       <c r="E37" s="6"/>
       <c r="F37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="8" t="s">
-        <v>67</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="16"/>
+        <v>65</v>
+      </c>
+      <c r="D38" s="17"/>
       <c r="E38" s="6"/>
       <c r="F38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
       <c r="E39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="16" t="n">
+        <v>67</v>
+      </c>
+      <c r="F39" s="17" t="n">
         <f aca="false">SUM(D35:D38)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
       <c r="E40" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F40" s="16" t="n">
+        <v>69</v>
+      </c>
+      <c r="F40" s="17" t="n">
         <f aca="false">F34+F39</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
+      <c r="A41" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
       <c r="E41" s="6"/>
       <c r="F41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
       <c r="E42" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F42" s="16" t="n">
+        <v>72</v>
+      </c>
+      <c r="F42" s="17" t="n">
         <f aca="false">MAX(F40 - F33,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
       <c r="E43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="16" t="n">
+        <v>74</v>
+      </c>
+      <c r="F43" s="17" t="n">
         <f aca="false">F42</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="C44" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="16" t="n">
+        <v>76</v>
+      </c>
+      <c r="D44" s="17" t="n">
         <f aca="false">F42-F43</f>
         <v>0</v>
       </c>
@@ -1230,45 +1229,45 @@
       <c r="F44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="A45" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
       <c r="E45" s="6"/>
       <c r="F45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
       <c r="E46" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F46" s="16" t="n">
+        <v>79</v>
+      </c>
+      <c r="F46" s="17" t="n">
         <f aca="false">F33-F40</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="19" t="s">
-        <v>83</v>
-      </c>
       <c r="C47" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D47" s="2"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>